<commit_message>
Integrated discord with streamlit
</commit_message>
<xml_diff>
--- a/market/market_changes.xlsx
+++ b/market/market_changes.xlsx
@@ -467,17 +467,17 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0442037580376271</v>
+        <v>0.01925380265402739</v>
       </c>
       <c r="C2" t="n">
-        <v>6630563705.644065</v>
+        <v>2888070398.104109</v>
       </c>
       <c r="D2" t="n">
-        <v>5435552278.504725</v>
+        <v>12342242302.91712</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-03-09T03:59:32.830188</t>
+          <t>2025-03-09T04:26:47.320735</t>
         </is>
       </c>
     </row>
@@ -488,17 +488,17 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8.657624341356542e-07</v>
+        <v>4.238788545257737e-07</v>
       </c>
       <c r="C3" t="n">
-        <v>36362022.23369747</v>
+        <v>17802911.89008249</v>
       </c>
       <c r="D3" t="n">
-        <v>15616511.11359374</v>
+        <v>46599258.27682871</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-03-09T03:59:32.830188</t>
+          <t>2025-03-09T04:26:47.320735</t>
         </is>
       </c>
     </row>
@@ -509,17 +509,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.479153384544496e-05</v>
+        <v>0.004240403655724095</v>
       </c>
       <c r="C4" t="n">
-        <v>26382213434.96708</v>
+        <v>2497597753221.492</v>
       </c>
       <c r="D4" t="n">
-        <v>5883318727.367015</v>
+        <v>4227602636016.839</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-03-09T03:59:32.830188</t>
+          <t>2025-03-09T04:26:47.320735</t>
         </is>
       </c>
     </row>
@@ -530,17 +530,17 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.05808437876573</v>
+        <v>1.112345263355795</v>
       </c>
       <c r="C5" t="n">
-        <v>105808437876.573</v>
+        <v>111234526335.5795</v>
       </c>
       <c r="D5" t="n">
-        <v>82664467571.21971</v>
+        <v>168272317101.9254</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-03-09T03:59:32.830188</t>
+          <t>2025-03-09T04:26:47.320735</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>178.0643661328804</v>
+        <v>228.1441865290555</v>
       </c>
       <c r="C6" t="n">
-        <v>2670965491993.206</v>
+        <v>3422162797935.833</v>
       </c>
       <c r="D6" t="n">
-        <v>942771872999.071</v>
+        <v>3544438988512.615</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-03-09T03:59:32.830188</t>
+          <t>2025-03-09T04:26:47.320735</t>
         </is>
       </c>
     </row>
@@ -572,17 +572,17 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>416.8082696377369</v>
+        <v>378.7045994700504</v>
       </c>
       <c r="C7" t="n">
-        <v>3092717360712.008</v>
+        <v>2809988128067.774</v>
       </c>
       <c r="D7" t="n">
-        <v>1117563590092.306</v>
+        <v>3565010145491.38</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-03-09T03:59:32.830188</t>
+          <t>2025-03-09T04:26:47.320735</t>
         </is>
       </c>
     </row>

</xml_diff>